<commit_message>
calibrate transp sector ships, rail, aviation
</commit_message>
<xml_diff>
--- a/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
+++ b/InputData/trans/AVLo/Avg Vehicle Loading.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anaxolt/Google Drive/2021/D.Development/TARGET_eps-us-3.2.1/InputData/trans/AVLo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\Mexico\eps-mexico\InputData\trans\AVLo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FE8474-B543-234B-8C9F-6B28AE5E40FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083876DC-CED2-4391-8BA7-A796EB208C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="500" windowWidth="26280" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10240" yWindow="410" windowWidth="14960" windowHeight="13130" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2534,7 +2534,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2719,6 +2719,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="41"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -3184,7 +3190,7 @@
     <xf numFmtId="168" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3274,6 +3280,9 @@
     </xf>
     <xf numFmtId="0" fontId="55" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="156">
     <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -3850,14 +3859,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="85.1640625" customWidth="1"/>
+    <col min="1" max="1" width="11.6328125" customWidth="1"/>
+    <col min="2" max="2" width="85.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4161,11 +4170,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="73.6640625" customWidth="1"/>
+    <col min="1" max="1" width="73.6328125" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="102.33203125" customWidth="1"/>
+    <col min="3" max="3" width="102.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4437,7 +4446,7 @@
         <v>33.023738872403563</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16">
+    <row r="36" spans="1:3">
       <c r="A36" s="10" t="s">
         <v>37</v>
       </c>
@@ -4608,7 +4617,7 @@
         <v>17287</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="16">
+    <row r="59" spans="1:3">
       <c r="A59" s="10" t="s">
         <v>47</v>
       </c>
@@ -4682,12 +4691,12 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="2" width="22.5" style="10" customWidth="1"/>
+    <col min="1" max="2" width="22.453125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="48">
+    <row r="1" spans="1:2" ht="43.5">
       <c r="A1" s="28" t="s">
         <v>135</v>
       </c>
@@ -4695,7 +4704,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="32">
+    <row r="2" spans="1:2" ht="29">
       <c r="A2" s="27" t="s">
         <v>133</v>
       </c>
@@ -4703,7 +4712,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16">
+    <row r="3" spans="1:2">
       <c r="A3" s="26" t="s">
         <v>131</v>
       </c>
@@ -4711,7 +4720,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16">
+    <row r="4" spans="1:2">
       <c r="A4" s="25"/>
       <c r="B4" s="25" t="s">
         <v>129</v>
@@ -4819,9 +4828,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.6328125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="16384" width="11.6640625" style="29"/>
+    <col min="1" max="16384" width="11.6328125" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -5049,11 +5058,11 @@
       <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="16" width="0" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" customHeight="1">
@@ -5766,16 +5775,16 @@
   <dimension ref="A1:AK7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="13.1796875" customWidth="1"/>
+    <col min="2" max="2" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="48">
+    <row r="1" spans="1:37" ht="43.5">
       <c r="A1" s="19" t="s">
         <v>101</v>
       </c>
@@ -6190,148 +6199,112 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9">
-        <f>'BTS NTS Modal Profile Data'!B8</f>
+      <c r="B4" s="53">
         <v>111.39416306433705</v>
       </c>
-      <c r="C4" s="7">
-        <f t="shared" ref="C4:C7" si="1">$B4</f>
+      <c r="C4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="D4" s="7">
-        <f t="shared" ref="D4:AK7" si="2">$B4</f>
+      <c r="D4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="E4" s="7">
-        <f t="shared" si="2"/>
+      <c r="E4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="F4" s="7">
-        <f t="shared" si="2"/>
+      <c r="F4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="G4" s="7">
-        <f t="shared" si="2"/>
+      <c r="G4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="H4" s="7">
-        <f t="shared" si="2"/>
+      <c r="H4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="I4" s="7">
-        <f t="shared" si="2"/>
+      <c r="I4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="J4" s="7">
-        <f t="shared" si="2"/>
+      <c r="J4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="K4" s="7">
-        <f t="shared" si="2"/>
+      <c r="K4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="L4" s="7">
-        <f t="shared" si="2"/>
+      <c r="L4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="M4" s="7">
-        <f t="shared" si="2"/>
+      <c r="M4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="N4" s="7">
-        <f t="shared" si="2"/>
+      <c r="N4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="O4" s="7">
-        <f t="shared" si="2"/>
+      <c r="O4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="P4" s="7">
-        <f t="shared" si="2"/>
+      <c r="P4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="Q4" s="7">
-        <f t="shared" si="2"/>
+      <c r="Q4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="R4" s="7">
-        <f t="shared" si="2"/>
+      <c r="R4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="S4" s="7">
-        <f t="shared" si="2"/>
+      <c r="S4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="T4" s="7">
-        <f t="shared" si="2"/>
+      <c r="T4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="U4" s="7">
-        <f t="shared" si="2"/>
+      <c r="U4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="V4" s="7">
-        <f t="shared" si="2"/>
+      <c r="V4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="W4" s="7">
-        <f t="shared" si="2"/>
+      <c r="W4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="X4" s="7">
-        <f t="shared" si="2"/>
+      <c r="X4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="Y4" s="7">
-        <f t="shared" si="2"/>
+      <c r="Y4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="Z4" s="7">
-        <f t="shared" si="2"/>
+      <c r="Z4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="AA4" s="7">
-        <f t="shared" si="2"/>
+      <c r="AA4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="AB4" s="7">
-        <f t="shared" si="2"/>
+      <c r="AB4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="AC4" s="7">
-        <f t="shared" si="2"/>
+      <c r="AC4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="AD4" s="7">
-        <f t="shared" si="2"/>
+      <c r="AD4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="AE4" s="7">
-        <f t="shared" si="2"/>
+      <c r="AE4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="AF4" s="7">
-        <f t="shared" si="2"/>
+      <c r="AF4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="AG4" s="7">
-        <f t="shared" si="2"/>
+      <c r="AG4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="AH4" s="7">
-        <f t="shared" si="2"/>
+      <c r="AH4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="AI4" s="7">
-        <f t="shared" si="2"/>
+      <c r="AI4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="AJ4" s="7">
-        <f t="shared" si="2"/>
+      <c r="AJ4" s="54">
         <v>111.39416306433705</v>
       </c>
-      <c r="AK4" s="7">
-        <f t="shared" si="2"/>
+      <c r="AK4" s="54">
         <v>111.39416306433705</v>
       </c>
     </row>
@@ -6339,296 +6312,225 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9">
-        <f>'BTS NTS Modal Profile Data'!B36</f>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="C5" s="7">
-        <f t="shared" si="1"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="D5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="E5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="F5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="G5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="H5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="I5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="J5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="K5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="L5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="M5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="N5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="O5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="P5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="Q5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="R5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="S5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="T5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="U5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="V5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="W5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="X5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="Y5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="Z5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="AA5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="AB5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="AC5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="AD5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="AE5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="AF5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="AG5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="AH5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="AI5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="AJ5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
-      </c>
-      <c r="AK5" s="7">
-        <f t="shared" si="2"/>
-        <v>48.656731685074099</v>
+      <c r="B5" s="53">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="C5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="D5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="E5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="F5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="G5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="H5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="I5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="J5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="K5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="L5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="M5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="N5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="O5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="P5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="Q5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="R5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="S5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="T5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="U5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="V5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="W5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="X5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="Y5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="Z5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AA5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AB5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AC5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AD5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AE5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AF5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AG5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AH5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AI5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AJ5" s="54">
+        <v>486.56731685074101</v>
+      </c>
+      <c r="AK5" s="54">
+        <v>486.56731685074101</v>
       </c>
     </row>
     <row r="6" spans="1:37">
       <c r="A6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="54">
         <v>1</v>
       </c>
-      <c r="C6" s="7">
-        <f t="shared" si="1"/>
+      <c r="C6" s="54">
         <v>1</v>
       </c>
-      <c r="D6" s="7">
-        <f t="shared" si="2"/>
+      <c r="D6" s="54">
         <v>1</v>
       </c>
-      <c r="E6" s="7">
-        <f t="shared" si="2"/>
+      <c r="E6" s="54">
         <v>1</v>
       </c>
-      <c r="F6" s="7">
-        <f t="shared" si="2"/>
+      <c r="F6" s="54">
         <v>1</v>
       </c>
-      <c r="G6" s="7">
-        <f t="shared" si="2"/>
+      <c r="G6" s="54">
         <v>1</v>
       </c>
-      <c r="H6" s="7">
-        <f t="shared" si="2"/>
+      <c r="H6" s="54">
         <v>1</v>
       </c>
-      <c r="I6" s="7">
-        <f t="shared" si="2"/>
+      <c r="I6" s="54">
         <v>1</v>
       </c>
-      <c r="J6" s="7">
-        <f t="shared" si="2"/>
+      <c r="J6" s="54">
         <v>1</v>
       </c>
-      <c r="K6" s="7">
-        <f t="shared" si="2"/>
+      <c r="K6" s="54">
         <v>1</v>
       </c>
-      <c r="L6" s="7">
-        <f t="shared" si="2"/>
+      <c r="L6" s="54">
         <v>1</v>
       </c>
-      <c r="M6" s="7">
-        <f t="shared" si="2"/>
+      <c r="M6" s="54">
         <v>1</v>
       </c>
-      <c r="N6" s="7">
-        <f t="shared" si="2"/>
+      <c r="N6" s="54">
         <v>1</v>
       </c>
-      <c r="O6" s="7">
-        <f t="shared" si="2"/>
+      <c r="O6" s="54">
         <v>1</v>
       </c>
-      <c r="P6" s="7">
-        <f t="shared" si="2"/>
+      <c r="P6" s="54">
         <v>1</v>
       </c>
-      <c r="Q6" s="7">
-        <f t="shared" si="2"/>
+      <c r="Q6" s="54">
         <v>1</v>
       </c>
-      <c r="R6" s="7">
-        <f t="shared" si="2"/>
+      <c r="R6" s="54">
         <v>1</v>
       </c>
-      <c r="S6" s="7">
-        <f t="shared" si="2"/>
+      <c r="S6" s="54">
         <v>1</v>
       </c>
-      <c r="T6" s="7">
-        <f t="shared" si="2"/>
+      <c r="T6" s="54">
         <v>1</v>
       </c>
-      <c r="U6" s="7">
-        <f t="shared" si="2"/>
+      <c r="U6" s="54">
         <v>1</v>
       </c>
-      <c r="V6" s="7">
-        <f t="shared" si="2"/>
+      <c r="V6" s="54">
         <v>1</v>
       </c>
-      <c r="W6" s="7">
-        <f t="shared" si="2"/>
+      <c r="W6" s="54">
         <v>1</v>
       </c>
-      <c r="X6" s="7">
-        <f t="shared" si="2"/>
+      <c r="X6" s="54">
         <v>1</v>
       </c>
-      <c r="Y6" s="7">
-        <f t="shared" si="2"/>
+      <c r="Y6" s="54">
         <v>1</v>
       </c>
-      <c r="Z6" s="7">
-        <f t="shared" si="2"/>
+      <c r="Z6" s="54">
         <v>1</v>
       </c>
-      <c r="AA6" s="7">
-        <f t="shared" si="2"/>
+      <c r="AA6" s="54">
         <v>1</v>
       </c>
-      <c r="AB6" s="7">
-        <f t="shared" si="2"/>
+      <c r="AB6" s="54">
         <v>1</v>
       </c>
-      <c r="AC6" s="7">
-        <f t="shared" si="2"/>
+      <c r="AC6" s="54">
         <v>1</v>
       </c>
-      <c r="AD6" s="7">
-        <f t="shared" si="2"/>
+      <c r="AD6" s="54">
         <v>1</v>
       </c>
-      <c r="AE6" s="7">
-        <f t="shared" si="2"/>
+      <c r="AE6" s="54">
         <v>1</v>
       </c>
-      <c r="AF6" s="7">
-        <f t="shared" si="2"/>
+      <c r="AF6" s="54">
         <v>1</v>
       </c>
-      <c r="AG6" s="7">
-        <f t="shared" si="2"/>
+      <c r="AG6" s="54">
         <v>1</v>
       </c>
-      <c r="AH6" s="7">
-        <f t="shared" si="2"/>
+      <c r="AH6" s="54">
         <v>1</v>
       </c>
-      <c r="AI6" s="7">
-        <f t="shared" si="2"/>
+      <c r="AI6" s="54">
         <v>1</v>
       </c>
-      <c r="AJ6" s="7">
-        <f t="shared" si="2"/>
+      <c r="AJ6" s="54">
         <v>1</v>
       </c>
-      <c r="AK6" s="7">
-        <f t="shared" si="2"/>
+      <c r="AK6" s="54">
         <v>1</v>
       </c>
     </row>
@@ -6641,11 +6543,11 @@
         <v>1.33</v>
       </c>
       <c r="C7" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C4:C7" si="1">$B7</f>
         <v>1.33</v>
       </c>
       <c r="D7" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D4:AK7" si="2">$B7</f>
         <v>1.33</v>
       </c>
       <c r="E7" s="7">
@@ -6793,16 +6695,16 @@
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="32">
+    <row r="1" spans="1:36" s="1" customFormat="1" ht="43.5">
       <c r="A1" s="19" t="s">
         <v>102</v>
       </c>
@@ -7205,144 +7107,109 @@
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6">
-        <f>'BTS NTS Modal Profile Data'!B9</f>
+      <c r="B4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="C4" s="6">
-        <f t="shared" si="0"/>
+      <c r="C4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="D4" s="6">
-        <f t="shared" si="1"/>
+      <c r="D4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="E4" s="6">
-        <f t="shared" si="1"/>
+      <c r="E4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="F4" s="6">
-        <f t="shared" si="1"/>
+      <c r="F4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="G4" s="6">
-        <f t="shared" si="1"/>
+      <c r="G4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="H4" s="6">
-        <f t="shared" si="1"/>
+      <c r="H4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="I4" s="6">
-        <f t="shared" si="1"/>
+      <c r="I4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="J4" s="6">
-        <f t="shared" si="1"/>
+      <c r="J4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="K4" s="6">
-        <f t="shared" si="1"/>
+      <c r="K4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="L4" s="6">
-        <f t="shared" si="1"/>
+      <c r="L4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="M4" s="6">
-        <f t="shared" si="1"/>
+      <c r="M4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="N4" s="6">
-        <f t="shared" si="1"/>
+      <c r="N4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="O4" s="6">
-        <f t="shared" si="1"/>
+      <c r="O4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="P4" s="6">
-        <f t="shared" si="1"/>
+      <c r="P4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="Q4" s="6">
-        <f t="shared" si="1"/>
+      <c r="Q4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="R4" s="6">
-        <f t="shared" si="1"/>
+      <c r="R4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="S4" s="6">
-        <f t="shared" si="1"/>
+      <c r="S4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="T4" s="6">
-        <f t="shared" si="1"/>
+      <c r="T4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="U4" s="6">
-        <f t="shared" si="1"/>
+      <c r="U4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="V4" s="6">
-        <f t="shared" si="1"/>
+      <c r="V4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="W4" s="6">
-        <f t="shared" si="1"/>
+      <c r="W4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="X4" s="6">
-        <f t="shared" si="1"/>
+      <c r="X4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="Y4" s="6">
-        <f t="shared" si="1"/>
+      <c r="Y4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="Z4" s="6">
-        <f t="shared" si="1"/>
+      <c r="Z4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="AA4" s="6">
-        <f t="shared" si="1"/>
+      <c r="AA4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="AB4" s="6">
-        <f t="shared" si="1"/>
+      <c r="AB4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="AC4" s="6">
-        <f t="shared" si="1"/>
+      <c r="AC4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="AD4" s="6">
-        <f t="shared" si="1"/>
+      <c r="AD4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="AE4" s="6">
-        <f t="shared" si="1"/>
+      <c r="AE4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="AF4" s="6">
-        <f t="shared" si="1"/>
+      <c r="AF4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="AG4" s="6">
-        <f t="shared" si="1"/>
+      <c r="AG4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="AH4" s="6">
-        <f t="shared" si="1"/>
+      <c r="AH4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="AI4" s="6">
-        <f t="shared" si="1"/>
+      <c r="AI4" s="55">
         <v>41.989116133258747</v>
       </c>
-      <c r="AJ4" s="6">
-        <f t="shared" si="1"/>
+      <c r="AJ4" s="55">
         <v>41.989116133258747</v>
       </c>
     </row>
@@ -7350,144 +7217,109 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6">
-        <f>'BTS NTS Modal Profile Data'!B19</f>
+      <c r="B5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="C5" s="6">
-        <f t="shared" si="0"/>
+      <c r="C5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="D5" s="6">
-        <f t="shared" si="1"/>
+      <c r="D5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="E5" s="6">
-        <f t="shared" si="1"/>
+      <c r="E5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="F5" s="6">
-        <f t="shared" si="1"/>
+      <c r="F5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="G5" s="6">
-        <f t="shared" si="1"/>
+      <c r="G5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="H5" s="6">
-        <f t="shared" si="1"/>
+      <c r="H5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="I5" s="6">
-        <f t="shared" si="1"/>
+      <c r="I5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="J5" s="6">
-        <f t="shared" si="1"/>
+      <c r="J5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="K5" s="6">
-        <f t="shared" si="1"/>
+      <c r="K5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="L5" s="6">
-        <f t="shared" si="1"/>
+      <c r="L5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="M5" s="6">
-        <f t="shared" si="1"/>
+      <c r="M5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="N5" s="6">
-        <f t="shared" si="1"/>
+      <c r="N5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="O5" s="6">
-        <f t="shared" si="1"/>
+      <c r="O5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="P5" s="6">
-        <f t="shared" si="1"/>
+      <c r="P5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="Q5" s="6">
-        <f t="shared" si="1"/>
+      <c r="Q5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="R5" s="6">
-        <f t="shared" si="1"/>
+      <c r="R5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="S5" s="6">
-        <f t="shared" si="1"/>
+      <c r="S5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="T5" s="6">
-        <f t="shared" si="1"/>
+      <c r="T5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="U5" s="6">
-        <f t="shared" si="1"/>
+      <c r="U5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="V5" s="6">
-        <f t="shared" si="1"/>
+      <c r="V5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="W5" s="6">
-        <f t="shared" si="1"/>
+      <c r="W5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="X5" s="6">
-        <f t="shared" si="1"/>
+      <c r="X5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="Y5" s="6">
-        <f t="shared" si="1"/>
+      <c r="Y5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="Z5" s="6">
-        <f t="shared" si="1"/>
+      <c r="Z5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="AA5" s="6">
-        <f t="shared" si="1"/>
+      <c r="AA5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="AB5" s="6">
-        <f t="shared" si="1"/>
+      <c r="AB5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="AC5" s="6">
-        <f t="shared" si="1"/>
+      <c r="AC5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="AD5" s="6">
-        <f t="shared" si="1"/>
+      <c r="AD5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="AE5" s="6">
-        <f t="shared" si="1"/>
+      <c r="AE5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="AF5" s="6">
-        <f t="shared" si="1"/>
+      <c r="AF5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="AG5" s="6">
-        <f t="shared" si="1"/>
+      <c r="AG5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="AH5" s="6">
-        <f t="shared" si="1"/>
+      <c r="AH5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="AI5" s="6">
-        <f t="shared" si="1"/>
+      <c r="AI5" s="55">
         <v>3512.35916421195</v>
       </c>
-      <c r="AJ5" s="6">
-        <f t="shared" si="1"/>
+      <c r="AJ5" s="55">
         <v>3512.35916421195</v>
       </c>
     </row>
@@ -7495,144 +7327,109 @@
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6">
-        <f>'BTS NTS Modal Profile Data'!B54</f>
+      <c r="B6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="C6" s="6">
-        <f t="shared" si="0"/>
+      <c r="C6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="D6" s="6">
-        <f t="shared" si="1"/>
+      <c r="D6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="E6" s="6">
-        <f t="shared" si="1"/>
+      <c r="E6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="F6" s="6">
-        <f t="shared" si="1"/>
+      <c r="F6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="G6" s="6">
-        <f t="shared" si="1"/>
+      <c r="G6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="H6" s="6">
-        <f t="shared" si="1"/>
+      <c r="H6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="I6" s="6">
-        <f t="shared" si="1"/>
+      <c r="I6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="J6" s="6">
-        <f t="shared" si="1"/>
+      <c r="J6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="K6" s="6">
-        <f t="shared" si="1"/>
+      <c r="K6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="L6" s="6">
-        <f t="shared" si="1"/>
+      <c r="L6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="M6" s="6">
-        <f t="shared" si="1"/>
+      <c r="M6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="N6" s="6">
-        <f t="shared" si="1"/>
+      <c r="N6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="O6" s="6">
-        <f t="shared" si="1"/>
+      <c r="O6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="P6" s="6">
-        <f t="shared" si="1"/>
+      <c r="P6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="Q6" s="6">
-        <f t="shared" si="1"/>
+      <c r="Q6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="R6" s="6">
-        <f t="shared" si="1"/>
+      <c r="R6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="S6" s="6">
-        <f t="shared" si="1"/>
+      <c r="S6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="T6" s="6">
-        <f t="shared" si="1"/>
+      <c r="T6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="U6" s="6">
-        <f t="shared" si="1"/>
+      <c r="U6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="V6" s="6">
-        <f t="shared" si="1"/>
+      <c r="V6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="W6" s="6">
-        <f t="shared" si="1"/>
+      <c r="W6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="X6" s="6">
-        <f t="shared" si="1"/>
+      <c r="X6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="Y6" s="6">
-        <f t="shared" si="1"/>
+      <c r="Y6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="Z6" s="6">
-        <f t="shared" si="1"/>
+      <c r="Z6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="AA6" s="6">
-        <f t="shared" si="1"/>
+      <c r="AA6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="AB6" s="6">
-        <f t="shared" si="1"/>
+      <c r="AB6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="AC6" s="6">
-        <f t="shared" si="1"/>
+      <c r="AC6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="AD6" s="6">
-        <f t="shared" si="1"/>
+      <c r="AD6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="AE6" s="6">
-        <f t="shared" si="1"/>
+      <c r="AE6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="AF6" s="6">
-        <f t="shared" si="1"/>
+      <c r="AF6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="AG6" s="6">
-        <f t="shared" si="1"/>
+      <c r="AG6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="AH6" s="6">
-        <f t="shared" si="1"/>
+      <c r="AH6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="AI6" s="6">
-        <f t="shared" si="1"/>
+      <c r="AI6" s="55">
         <v>1974.4736422180429</v>
       </c>
-      <c r="AJ6" s="6">
-        <f t="shared" si="1"/>
+      <c r="AJ6" s="55">
         <v>1974.4736422180429</v>
       </c>
     </row>

</xml_diff>